<commit_message>
add java hook IO
</commit_message>
<xml_diff>
--- a/bin-java/WEB-INF/resources/Java知识点整理.xlsx
+++ b/bin-java/WEB-INF/resources/Java知识点整理.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20040" windowHeight="16000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
     <sheet name="java容器" sheetId="3" r:id="rId2"/>
     <sheet name="线程" sheetId="2" r:id="rId3"/>
+    <sheet name="IO" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>容器</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,10 +95,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>读写文件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Jprofile/Yourkit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -216,6 +213,18 @@
   </si>
   <si>
     <t>都是旧的类，内部实现都是Synchronized的，慢一些，现在基本不用了。</t>
+  </si>
+  <si>
+    <t>输入/输出流</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>常见的节点流和处理流</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文件流、缓冲流、数据流、转换流、Print流、Object流</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -312,7 +321,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -327,15 +336,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="超链接" xfId="2" builtinId="8" hidden="1"/>
@@ -862,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -881,7 +893,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -889,7 +901,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="6"/>
+      <c r="A3" s="11"/>
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -898,7 +910,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="6"/>
+      <c r="A4" s="11"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1"/>
@@ -910,7 +922,7 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -918,13 +930,13 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="6"/>
+      <c r="A7" s="11"/>
       <c r="B7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="6"/>
+      <c r="A8" s="11"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1"/>
@@ -936,7 +948,7 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B10" t="s">
@@ -944,42 +956,42 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="11"/>
+      <c r="B12" s="9"/>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" ht="30">
+      <c r="A13" s="11"/>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="11"/>
+      <c r="B14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" ht="30">
-      <c r="A13" s="6"/>
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="6"/>
-      <c r="B14" t="s">
+      <c r="D14" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -992,7 +1004,7 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B16" t="s">
@@ -1000,7 +1012,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="6"/>
+      <c r="A17" s="11"/>
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -1015,27 +1027,27 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="6" t="s">
-        <v>41</v>
+      <c r="A19" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="B19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="11"/>
+      <c r="B20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="6"/>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-    </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="6"/>
+      <c r="A21" s="11"/>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="6"/>
+      <c r="A22" s="11"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1"/>
@@ -1048,77 +1060,89 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="6"/>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="6"/>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" t="s">
+    <row r="29" spans="1:7">
+      <c r="A29" s="11"/>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="11"/>
+      <c r="B32" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="6"/>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="6"/>
-      <c r="B30" t="s">
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="B31" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:D13"/>
-    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1143,15 +1167,15 @@
   <sheetData>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
         <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1185,50 +1209,50 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
         <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
         <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1241,4 +1265,22 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>